<commit_message>
Fix-bug del numero de bloque que esta modificado para el Write-back
Pasa la prueba de escribir un bloque modificado, antes de caerle encima
con el que se ocupa
</commit_message>
<xml_diff>
--- a/Memoria.xlsx
+++ b/Memoria.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="964" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -127,10 +127,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C3:G356"/>
+  <dimension ref="C3:L356"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D100" activeCellId="0" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1984,6 +1984,10 @@
         <f aca="false">MOD(D99,4)</f>
         <v>3</v>
       </c>
+      <c r="L99" s="0" t="n">
+        <f aca="false">24*4</f>
+        <v>96</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="n">
@@ -6873,8 +6877,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>